<commit_message>
Add test cases and description
</commit_message>
<xml_diff>
--- a/Lab_4/TestCases.xlsx
+++ b/Lab_4/TestCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SHIT\Third course\Program testing\Labwork_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SHIT\Third course\Program testing\Lab_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{279F8399-711E-40D2-872A-4AFB39954D5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0725FA46-9548-4005-BC73-5E1196FC8E4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{93228DF9-C513-44B6-A871-163F25800BDD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
   <si>
     <r>
       <t>System Name</t>
@@ -121,9 +121,6 @@
     <t>1: Start the program; 2: Enter a number</t>
   </si>
   <si>
-    <t>Exception</t>
-  </si>
-  <si>
     <t>1. Сheck for incorrectly entered data</t>
   </si>
   <si>
@@ -188,13 +185,67 @@
   </si>
   <si>
     <t>2-341</t>
+  </si>
+  <si>
+    <t>2. Check for correct calculations</t>
+  </si>
+  <si>
+    <t>TC11</t>
+  </si>
+  <si>
+    <t>TC12</t>
+  </si>
+  <si>
+    <t>TC13</t>
+  </si>
+  <si>
+    <t>TC14</t>
+  </si>
+  <si>
+    <t>TC15</t>
+  </si>
+  <si>
+    <t>TC16</t>
+  </si>
+  <si>
+    <t>TC17</t>
+  </si>
+  <si>
+    <t>Сheck the correctness of the calculations of the first formula</t>
+  </si>
+  <si>
+    <t>1: Staty the program; 2: Enter a number</t>
+  </si>
+  <si>
+    <t>2.2 Check second formula</t>
+  </si>
+  <si>
+    <t>2.1 Check first formula</t>
+  </si>
+  <si>
+    <t>2.3 Check third formula</t>
+  </si>
+  <si>
+    <t>2.4 Check fourth formula</t>
+  </si>
+  <si>
+    <t>Сheck the correctness of the calculations of the fourth formula</t>
+  </si>
+  <si>
+    <t>Сheck the correctness of the calculations of the third formula</t>
+  </si>
+  <si>
+    <t>Exception: Invalid data</t>
+  </si>
+  <si>
+    <t>Exception:You have some errors with typing your number, enter a number between 2.934 and 101.89!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,8 +301,14 @@
       <name val="MS Gothic"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +333,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -471,7 +534,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -503,38 +566,44 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A74E413B-3E71-496C-B0F3-849E25E0FC21}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="B62" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -864,7 +933,7 @@
     <col min="2" max="2" width="53.6640625" customWidth="1"/>
     <col min="3" max="3" width="35.44140625" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="82.88671875" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="17.5546875" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" customWidth="1"/>
@@ -884,21 +953,21 @@
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
@@ -929,42 +998,42 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="A8" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:8" ht="14.4" customHeight="1">
       <c r="A9" t="s">
@@ -980,15 +1049,15 @@
         <v>-234</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -997,15 +1066,15 @@
         <v>1.2</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -1014,135 +1083,608 @@
         <v>101.99</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
       <c r="D12">
-        <v>101.89</v>
+        <v>101.9</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
       </c>
       <c r="D13">
-        <v>2.9340000000000002</v>
+        <v>2.9329999999999998</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
         <v>36</v>
       </c>
-      <c r="C14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" t="s">
-        <v>37</v>
-      </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
         <v>38</v>
       </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="13">
+        <v>2345</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
         <v>42</v>
       </c>
-      <c r="D16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="22">
-        <v>2345</v>
-      </c>
-      <c r="E17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E18" t="s">
-        <v>21</v>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="12"/>
+      <c r="B20" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21">
+        <v>101.89</v>
+      </c>
+      <c r="E21">
+        <v>2111616.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22">
+        <v>2.9340000000000002</v>
+      </c>
+      <c r="E22">
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24">
+        <v>50</v>
+      </c>
+      <c r="E24">
+        <v>245230.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25">
+        <v>100</v>
+      </c>
+      <c r="E25">
+        <v>1995637.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26">
+        <v>100.82340000000001</v>
+      </c>
+      <c r="E26">
+        <v>2045628.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27">
+        <v>18.364799999999999</v>
+      </c>
+      <c r="E27">
+        <v>11471</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="B28" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29">
+        <v>101.89</v>
+      </c>
+      <c r="E29">
+        <v>2272238.2999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30">
+        <v>2.9340000000000002</v>
+      </c>
+      <c r="E30">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>56.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32">
+        <v>50</v>
+      </c>
+      <c r="E32">
+        <v>265957.3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33">
+        <v>100</v>
+      </c>
+      <c r="E33">
+        <v>2147739.6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34">
+        <v>100.82340000000001</v>
+      </c>
+      <c r="E34">
+        <v>2201404.1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35">
+        <v>18.364799999999999</v>
+      </c>
+      <c r="E35">
+        <v>12805.7</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37">
+        <v>101.89</v>
+      </c>
+      <c r="E37">
+        <v>20815.8</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38">
+        <v>2.9340000000000002</v>
+      </c>
+      <c r="E38">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40">
+        <v>50</v>
+      </c>
+      <c r="E40">
+        <v>5090.75</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41">
+        <v>100</v>
+      </c>
+      <c r="E41">
+        <v>20056.5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="B42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42">
+        <v>100.82340000000001</v>
+      </c>
+      <c r="E42">
+        <v>20385.599999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="B43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43">
+        <v>18.364799999999999</v>
+      </c>
+      <c r="E43">
+        <v>722.3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="B44" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45">
+        <v>101.89</v>
+      </c>
+      <c r="E45">
+        <v>422.8</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7">
+      <c r="B46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46">
+        <v>2.9340000000000002</v>
+      </c>
+      <c r="E46">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="B47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7">
+      <c r="B48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48">
+        <v>50</v>
+      </c>
+      <c r="E48">
+        <v>207.5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="B49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49">
+        <v>100</v>
+      </c>
+      <c r="E49">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5">
+      <c r="B50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50">
+        <v>100.82340000000001</v>
+      </c>
+      <c r="E50">
+        <v>418.4</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5">
+      <c r="B51" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51">
+        <v>18.364799999999999</v>
+      </c>
+      <c r="E51">
+        <v>76.2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="9">
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B36:G36"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A19:H19"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="D15" twoDigitTextYear="1"/>

</xml_diff>

<commit_message>
Add test cases and subscription
</commit_message>
<xml_diff>
--- a/Lab_4/TestCases.xlsx
+++ b/Lab_4/TestCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SHIT\Third course\Program testing\Labwork_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SHIT\Third course\Program testing\Lab_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{279F8399-711E-40D2-872A-4AFB39954D5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0725FA46-9548-4005-BC73-5E1196FC8E4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{93228DF9-C513-44B6-A871-163F25800BDD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
   <si>
     <r>
       <t>System Name</t>
@@ -121,9 +121,6 @@
     <t>1: Start the program; 2: Enter a number</t>
   </si>
   <si>
-    <t>Exception</t>
-  </si>
-  <si>
     <t>1. Сheck for incorrectly entered data</t>
   </si>
   <si>
@@ -188,13 +185,67 @@
   </si>
   <si>
     <t>2-341</t>
+  </si>
+  <si>
+    <t>2. Check for correct calculations</t>
+  </si>
+  <si>
+    <t>TC11</t>
+  </si>
+  <si>
+    <t>TC12</t>
+  </si>
+  <si>
+    <t>TC13</t>
+  </si>
+  <si>
+    <t>TC14</t>
+  </si>
+  <si>
+    <t>TC15</t>
+  </si>
+  <si>
+    <t>TC16</t>
+  </si>
+  <si>
+    <t>TC17</t>
+  </si>
+  <si>
+    <t>Сheck the correctness of the calculations of the first formula</t>
+  </si>
+  <si>
+    <t>1: Staty the program; 2: Enter a number</t>
+  </si>
+  <si>
+    <t>2.2 Check second formula</t>
+  </si>
+  <si>
+    <t>2.1 Check first formula</t>
+  </si>
+  <si>
+    <t>2.3 Check third formula</t>
+  </si>
+  <si>
+    <t>2.4 Check fourth formula</t>
+  </si>
+  <si>
+    <t>Сheck the correctness of the calculations of the fourth formula</t>
+  </si>
+  <si>
+    <t>Сheck the correctness of the calculations of the third formula</t>
+  </si>
+  <si>
+    <t>Exception: Invalid data</t>
+  </si>
+  <si>
+    <t>Exception:You have some errors with typing your number, enter a number between 2.934 and 101.89!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,8 +301,14 @@
       <name val="MS Gothic"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +333,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -471,7 +534,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -503,38 +566,44 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A74E413B-3E71-496C-B0F3-849E25E0FC21}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="B62" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -864,7 +933,7 @@
     <col min="2" max="2" width="53.6640625" customWidth="1"/>
     <col min="3" max="3" width="35.44140625" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="82.88671875" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="17.5546875" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" customWidth="1"/>
@@ -884,21 +953,21 @@
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
@@ -929,42 +998,42 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="A8" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:8" ht="14.4" customHeight="1">
       <c r="A9" t="s">
@@ -980,15 +1049,15 @@
         <v>-234</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -997,15 +1066,15 @@
         <v>1.2</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -1014,135 +1083,608 @@
         <v>101.99</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
       <c r="D12">
-        <v>101.89</v>
+        <v>101.9</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
       </c>
       <c r="D13">
-        <v>2.9340000000000002</v>
+        <v>2.9329999999999998</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
         <v>36</v>
       </c>
-      <c r="C14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" t="s">
-        <v>37</v>
-      </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
         <v>38</v>
       </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="13">
+        <v>2345</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
         <v>42</v>
       </c>
-      <c r="D16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="22">
-        <v>2345</v>
-      </c>
-      <c r="E17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E18" t="s">
-        <v>21</v>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="12"/>
+      <c r="B20" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21">
+        <v>101.89</v>
+      </c>
+      <c r="E21">
+        <v>2111616.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22">
+        <v>2.9340000000000002</v>
+      </c>
+      <c r="E22">
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24">
+        <v>50</v>
+      </c>
+      <c r="E24">
+        <v>245230.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25">
+        <v>100</v>
+      </c>
+      <c r="E25">
+        <v>1995637.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26">
+        <v>100.82340000000001</v>
+      </c>
+      <c r="E26">
+        <v>2045628.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27">
+        <v>18.364799999999999</v>
+      </c>
+      <c r="E27">
+        <v>11471</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="B28" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29">
+        <v>101.89</v>
+      </c>
+      <c r="E29">
+        <v>2272238.2999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30">
+        <v>2.9340000000000002</v>
+      </c>
+      <c r="E30">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>56.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32">
+        <v>50</v>
+      </c>
+      <c r="E32">
+        <v>265957.3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33">
+        <v>100</v>
+      </c>
+      <c r="E33">
+        <v>2147739.6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34">
+        <v>100.82340000000001</v>
+      </c>
+      <c r="E34">
+        <v>2201404.1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35">
+        <v>18.364799999999999</v>
+      </c>
+      <c r="E35">
+        <v>12805.7</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37">
+        <v>101.89</v>
+      </c>
+      <c r="E37">
+        <v>20815.8</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38">
+        <v>2.9340000000000002</v>
+      </c>
+      <c r="E38">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40">
+        <v>50</v>
+      </c>
+      <c r="E40">
+        <v>5090.75</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41">
+        <v>100</v>
+      </c>
+      <c r="E41">
+        <v>20056.5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="B42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42">
+        <v>100.82340000000001</v>
+      </c>
+      <c r="E42">
+        <v>20385.599999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="B43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43">
+        <v>18.364799999999999</v>
+      </c>
+      <c r="E43">
+        <v>722.3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="B44" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45">
+        <v>101.89</v>
+      </c>
+      <c r="E45">
+        <v>422.8</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7">
+      <c r="B46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46">
+        <v>2.9340000000000002</v>
+      </c>
+      <c r="E46">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="B47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7">
+      <c r="B48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48">
+        <v>50</v>
+      </c>
+      <c r="E48">
+        <v>207.5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="B49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49">
+        <v>100</v>
+      </c>
+      <c r="E49">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5">
+      <c r="B50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50">
+        <v>100.82340000000001</v>
+      </c>
+      <c r="E50">
+        <v>418.4</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5">
+      <c r="B51" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51">
+        <v>18.364799999999999</v>
+      </c>
+      <c r="E51">
+        <v>76.2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="9">
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B36:G36"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A19:H19"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="D15" twoDigitTextYear="1"/>

</xml_diff>